<commit_message>
chore: update db.example.xlsx + some minor adjustments
</commit_message>
<xml_diff>
--- a/db.example.xlsx
+++ b/db.example.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Entidades" sheetId="1" r:id="rId1"/>
     <sheet name="Nota Fiscal" sheetId="2" r:id="rId2"/>
     <sheet name="Dados de Produtos e Serviços NF" sheetId="3" r:id="rId3"/>
+    <sheet name="Dados das listas" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="167">
   <si>
     <t>tipo</t>
   </si>
@@ -33,6 +34,9 @@
     <t>nome</t>
   </si>
   <si>
+    <t>Produtor Rural</t>
+  </si>
+  <si>
     <t>natureza da operação</t>
   </si>
   <si>
@@ -57,10 +61,7 @@
     <t>destinatário</t>
   </si>
   <si>
-    <t>não</t>
-  </si>
-  <si>
-    <t>sim</t>
+    <t>Venda</t>
   </si>
   <si>
     <t>grupo</t>
@@ -96,16 +97,427 @@
     <t>CB</t>
   </si>
   <si>
-    <t>(de acordo com a coluna "número")</t>
-  </si>
-  <si>
-    <t>venda</t>
-  </si>
-  <si>
-    <t>Produtor rural</t>
-  </si>
-  <si>
-    <t>(Opcional)</t>
+    <t>contribuinte icms</t>
+  </si>
+  <si>
+    <t>tipos de entidade</t>
+  </si>
+  <si>
+    <t>Inscrição Estadual</t>
+  </si>
+  <si>
+    <t>Protocolo</t>
+  </si>
+  <si>
+    <t>Contabilista Pessoa Física</t>
+  </si>
+  <si>
+    <t>Gráfica e Outros - CNPJ</t>
+  </si>
+  <si>
+    <t>Despachante Aduaneiro Pessoa Física</t>
+  </si>
+  <si>
+    <t>Recinto Alfandegado Pessoa Jurídica</t>
+  </si>
+  <si>
+    <t>CERM/TFRM Pessoa Física</t>
+  </si>
+  <si>
+    <t>CERM/TFRM Pessoa Jurídica</t>
+  </si>
+  <si>
+    <t>VAF Especial</t>
+  </si>
+  <si>
+    <t>Contribuinte Interestadual</t>
+  </si>
+  <si>
+    <t>Pessoa Física Autuada - PTA eletrônico</t>
+  </si>
+  <si>
+    <t>Responsável Tributário - Instituição Financeira</t>
+  </si>
+  <si>
+    <t>Conselheiro</t>
+  </si>
+  <si>
+    <t>Adubo</t>
+  </si>
+  <si>
+    <t>Algodão</t>
+  </si>
+  <si>
+    <t>Animais silvestres</t>
+  </si>
+  <si>
+    <t>Apicultura</t>
+  </si>
+  <si>
+    <t>Aquicultura e pesca</t>
+  </si>
+  <si>
+    <t>Avicultura - ovos</t>
+  </si>
+  <si>
+    <t>Avicultura - reprodutor</t>
+  </si>
+  <si>
+    <t>Avicultura para corte</t>
+  </si>
+  <si>
+    <t>Avicultura para recria</t>
+  </si>
+  <si>
+    <t>Café</t>
+  </si>
+  <si>
+    <t>Cana de açucar</t>
+  </si>
+  <si>
+    <t>Carvão de floresta nativa</t>
+  </si>
+  <si>
+    <t>Carvão de floresta plantada</t>
+  </si>
+  <si>
+    <t>Carvão mineral</t>
+  </si>
+  <si>
+    <t>Cereais</t>
+  </si>
+  <si>
+    <t>Combustíveis</t>
+  </si>
+  <si>
+    <t>Derivados do leite</t>
+  </si>
+  <si>
+    <t>Dormentes</t>
+  </si>
+  <si>
+    <t>Embrião asinino</t>
+  </si>
+  <si>
+    <t>Embrião bovino</t>
+  </si>
+  <si>
+    <t>Embrião bufalino</t>
+  </si>
+  <si>
+    <t>Embrião caprino</t>
+  </si>
+  <si>
+    <t>Embrião equino</t>
+  </si>
+  <si>
+    <t>Embrião muar</t>
+  </si>
+  <si>
+    <t>Embrião ovino</t>
+  </si>
+  <si>
+    <t>Embrião suíno</t>
+  </si>
+  <si>
+    <t>Embrião taurino</t>
+  </si>
+  <si>
+    <t>Esterco animal</t>
+  </si>
+  <si>
+    <t>Farelos</t>
+  </si>
+  <si>
+    <t>Feno</t>
+  </si>
+  <si>
+    <t>Flores</t>
+  </si>
+  <si>
+    <t>Gado asinino - reprodutor</t>
+  </si>
+  <si>
+    <t>Gado asinino para corte</t>
+  </si>
+  <si>
+    <t>Gado asinino para recria</t>
+  </si>
+  <si>
+    <t>Gado asinino para serviço</t>
+  </si>
+  <si>
+    <t>Gado bufalino - reprodutor</t>
+  </si>
+  <si>
+    <t>Gado bufalino para corte</t>
+  </si>
+  <si>
+    <t>Gado bufalino para recria</t>
+  </si>
+  <si>
+    <t>Gado bufalino para serviço</t>
+  </si>
+  <si>
+    <t>Gado caprinos vivos</t>
+  </si>
+  <si>
+    <t>Gado equino - reprodutor</t>
+  </si>
+  <si>
+    <t>Gado equino para corte</t>
+  </si>
+  <si>
+    <t>Gado equino para recria</t>
+  </si>
+  <si>
+    <t>Gado equino para serviço</t>
+  </si>
+  <si>
+    <t>Gado muar - reprodutor</t>
+  </si>
+  <si>
+    <t>Gado muar para corte</t>
+  </si>
+  <si>
+    <t>Gado muar para recria</t>
+  </si>
+  <si>
+    <t>Gado muar para serviço</t>
+  </si>
+  <si>
+    <t>Gado suino - reprodutor</t>
+  </si>
+  <si>
+    <t>Gado suino para corte</t>
+  </si>
+  <si>
+    <t>Gado suino para recria</t>
+  </si>
+  <si>
+    <t>Gado taurino - reprodutor</t>
+  </si>
+  <si>
+    <t>Gado taurino para corte</t>
+  </si>
+  <si>
+    <t>Gado taurino para recria</t>
+  </si>
+  <si>
+    <t>Gado taurino para serviço</t>
+  </si>
+  <si>
+    <t>Hortifrutigranjeiros</t>
+  </si>
+  <si>
+    <t>Leite</t>
+  </si>
+  <si>
+    <t>Lenha - floresta nativa</t>
+  </si>
+  <si>
+    <t>Lenha - floresta plantada</t>
+  </si>
+  <si>
+    <t>Madeira</t>
+  </si>
+  <si>
+    <t>Milho</t>
+  </si>
+  <si>
+    <t>Minerais</t>
+  </si>
+  <si>
+    <t>Mudança</t>
+  </si>
+  <si>
+    <t>Mudas e sementes</t>
+  </si>
+  <si>
+    <t>Outros</t>
+  </si>
+  <si>
+    <t>Ovinocultura</t>
+  </si>
+  <si>
+    <t>Palha de café</t>
+  </si>
+  <si>
+    <t>Piscicultura - reprodutor</t>
+  </si>
+  <si>
+    <t>Piscicultura para corte</t>
+  </si>
+  <si>
+    <t>Piscicultura para recria</t>
+  </si>
+  <si>
+    <t>Prestação de serviço de transporte</t>
+  </si>
+  <si>
+    <t>Queijo artesanal</t>
+  </si>
+  <si>
+    <t>Ração</t>
+  </si>
+  <si>
+    <t>Resíduos</t>
+  </si>
+  <si>
+    <t>Semem</t>
+  </si>
+  <si>
+    <t>Soja</t>
+  </si>
+  <si>
+    <t>Sorgos</t>
+  </si>
+  <si>
+    <t>Suplementos</t>
+  </si>
+  <si>
+    <t>Estrangeira - Importação direta</t>
+  </si>
+  <si>
+    <t>Estrangeira - Adquirida no mercado interno</t>
+  </si>
+  <si>
+    <t>unidades de medida - itens NF</t>
+  </si>
+  <si>
+    <t>origens - itens NF</t>
+  </si>
+  <si>
+    <t>grupos - itens NF</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>CX</t>
+  </si>
+  <si>
+    <t>DUZIA</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>JOGO</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>KM</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>MDC</t>
+  </si>
+  <si>
+    <t>METRO</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>PARES</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>QUILAT</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>TON</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>Gado bovino - reprodutor</t>
+  </si>
+  <si>
+    <t>Gado bovino para recria</t>
+  </si>
+  <si>
+    <t>Gado bovino para serviço</t>
+  </si>
+  <si>
+    <t>gado bovino para corte</t>
+  </si>
+  <si>
+    <t>naturezas de operação -NF</t>
+  </si>
+  <si>
+    <t>VENDA</t>
+  </si>
+  <si>
+    <t>REMESSA</t>
+  </si>
+  <si>
+    <t>CFOPS - NF</t>
+  </si>
+  <si>
+    <t>5102</t>
+  </si>
+  <si>
+    <t>5103</t>
+  </si>
+  <si>
+    <t>5105</t>
+  </si>
+  <si>
+    <t>5111</t>
+  </si>
+  <si>
+    <t>5113</t>
+  </si>
+  <si>
+    <t>5116</t>
+  </si>
+  <si>
+    <t>5118</t>
+  </si>
+  <si>
+    <t>5122</t>
+  </si>
+  <si>
+    <t>5159</t>
+  </si>
+  <si>
+    <t>5160</t>
+  </si>
+  <si>
+    <t>5401</t>
+  </si>
+  <si>
+    <t>5402</t>
+  </si>
+  <si>
+    <t>5551</t>
   </si>
 </sst>
 </file>
@@ -468,22 +880,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="33.7109375" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,29 +911,45 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Dados das listas'!$A$2:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,67 +960,80 @@
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="8" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="B2" s="2">
+        <v>5101</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Dados das listas'!$E$2:$E$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Dados das listas'!$F$2:$F$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +1041,7 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
@@ -634,7 +1075,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>149</v>
       </c>
       <c r="B2" s="2"/>
       <c r="D2" t="s">
@@ -647,7 +1088,666 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Dados das listas'!$B$2:$B$83</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Dados das listas'!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Dados das listas'!$D$2:$D$24</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F83"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>136</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>138</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: handle missing db cases
- a user friendly message is displayed when this exeption is raised
</commit_message>
<xml_diff>
--- a/db.example.xlsx
+++ b/db.example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Entidades" sheetId="1" r:id="rId1"/>
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,7 +1079,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,8 +1173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H4" sqref="G1:H4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: prepare for accepting recipient without IE
- validate if recipient has IE or Adress info, they must have at least
  one of them
- skip invoices having invalid recipients and display error message
- update db.example for holding the new fields
</commit_message>
<xml_diff>
--- a/db.example.xlsx
+++ b/db.example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Entidades" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="181">
   <si>
     <t>tipo</t>
   </si>
@@ -532,13 +532,34 @@
     <t>senha</t>
   </si>
   <si>
-    <t>[inscrição municipal]</t>
-  </si>
-  <si>
     <t>[apenas para controle próprio]</t>
   </si>
   <si>
     <t>[cpf/cnpj]</t>
+  </si>
+  <si>
+    <t>cep</t>
+  </si>
+  <si>
+    <t>bairro</t>
+  </si>
+  <si>
+    <t>logradouro (tipo)</t>
+  </si>
+  <si>
+    <t>logradouro (nome)</t>
+  </si>
+  <si>
+    <t>Avenida</t>
+  </si>
+  <si>
+    <t>Rua</t>
+  </si>
+  <si>
+    <t>Estrada</t>
+  </si>
+  <si>
+    <t>inscrição estadual</t>
   </si>
 </sst>
 </file>
@@ -909,28 +930,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="2" max="3" width="17.140625" customWidth="1"/>
     <col min="4" max="4" width="33.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="5" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>180</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -944,40 +966,53 @@
       <c r="F1" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>171</v>
-      </c>
+      <c r="G1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
       <c r="C2" s="4"/>
       <c r="D2" s="3"/>
       <c r="E2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
     </row>
   </sheetData>
@@ -985,12 +1020,18 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Dados das listas'!$A$2:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>A2:A5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Dados das listas'!$I$2:$I$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1052,10 +1093,10 @@
       <c r="B2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1115,7 +1156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1220,10 +1261,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I1" sqref="I1:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,9 +1277,10 @@
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1263,8 +1305,11 @@
       <c r="H1" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1289,8 +1334,11 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1315,8 +1363,11 @@
       <c r="H3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1335,8 +1386,11 @@
       <c r="G4" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1350,7 +1404,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1364,7 +1418,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1378,7 +1432,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1392,7 +1446,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1406,7 +1460,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1420,7 +1474,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1434,7 +1488,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1448,7 +1502,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1462,7 +1516,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1476,7 +1530,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1490,7 +1544,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
feat: add support for optional invoice extra notes
</commit_message>
<xml_diff>
--- a/db.example.xlsx
+++ b/db.example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Entidades" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="182">
   <si>
     <t>tipo</t>
   </si>
@@ -560,6 +560,9 @@
   </si>
   <si>
     <t>inscrição estadual</t>
+  </si>
+  <si>
+    <t>informações complementares</t>
   </si>
 </sst>
 </file>
@@ -932,7 +935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -1041,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,9 +1061,10 @@
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1088,8 +1092,11 @@
       <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="4" t="s">
@@ -1099,19 +1106,19 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="4"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="4"/>

</xml_diff>

<commit_message>
feat: populate db.example with sample dummy data
</commit_message>
<xml_diff>
--- a/db.example.xlsx
+++ b/db.example.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="199">
   <si>
     <t xml:space="preserve">tipo</t>
   </si>
@@ -58,7 +58,43 @@
     <t xml:space="preserve">número</t>
   </si>
   <si>
-    <t xml:space="preserve">[apenas para controle próprio]</t>
+    <t xml:space="preserve">Produtor Rural</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">456123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remetente 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">senhaforte123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">654321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destinatário 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">987654</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destinatário 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">centro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">direita</t>
   </si>
   <si>
     <t xml:space="preserve">natureza da operação</t>
@@ -91,7 +127,31 @@
     <t xml:space="preserve">informações complementares</t>
   </si>
   <si>
-    <t xml:space="preserve">[cpf/cnpj]</t>
+    <t xml:space="preserve">VENDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n-123456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">não</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">um comentário qualquer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n-789456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isento</t>
   </si>
   <si>
     <t xml:space="preserve">grupo</t>
@@ -118,6 +178,42 @@
     <t xml:space="preserve">NF</t>
   </si>
   <si>
+    <t xml:space="preserve">Café</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pó</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nacional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gado bovino para corte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fêmea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gado bovino para recria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gado bufalino - reprodutor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gado equino para corte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">macho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soja</t>
+  </si>
+  <si>
     <t xml:space="preserve">tipos de entidade</t>
   </si>
   <si>
@@ -142,24 +238,9 @@
     <t xml:space="preserve">campo booleano</t>
   </si>
   <si>
-    <t xml:space="preserve">Produtor Rural</t>
-  </si>
-  <si>
     <t xml:space="preserve">Adubo</t>
   </si>
   <si>
-    <t xml:space="preserve">Nacional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VENDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sim</t>
-  </si>
-  <si>
     <t xml:space="preserve">Avenida</t>
   </si>
   <si>
@@ -181,12 +262,6 @@
     <t xml:space="preserve">5102</t>
   </si>
   <si>
-    <t xml:space="preserve">não</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rua</t>
-  </si>
-  <si>
     <t xml:space="preserve">Protocolo</t>
   </si>
   <si>
@@ -202,9 +277,6 @@
     <t xml:space="preserve">5103</t>
   </si>
   <si>
-    <t xml:space="preserve">isento</t>
-  </si>
-  <si>
     <t xml:space="preserve">Estrada</t>
   </si>
   <si>
@@ -262,9 +334,6 @@
     <t xml:space="preserve">Avicultura para corte</t>
   </si>
   <si>
-    <t xml:space="preserve">KG</t>
-  </si>
-  <si>
     <t xml:space="preserve">5118</t>
   </si>
   <si>
@@ -283,9 +352,6 @@
     <t xml:space="preserve">VAF Especial</t>
   </si>
   <si>
-    <t xml:space="preserve">Café</t>
-  </si>
-  <si>
     <t xml:space="preserve">LT</t>
   </si>
   <si>
@@ -433,18 +499,9 @@
     <t xml:space="preserve">Gado bovino - reprodutor</t>
   </si>
   <si>
-    <t xml:space="preserve">Gado bovino para corte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gado bovino para recria</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gado bovino para serviço</t>
   </si>
   <si>
-    <t xml:space="preserve">Gado bufalino - reprodutor</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gado bufalino para corte</t>
   </si>
   <si>
@@ -460,9 +517,6 @@
     <t xml:space="preserve">Gado equino - reprodutor</t>
   </si>
   <si>
-    <t xml:space="preserve">Gado equino para corte</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gado equino para recria</t>
   </si>
   <si>
@@ -560,9 +614,6 @@
   </si>
   <si>
     <t xml:space="preserve">Semem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soja</t>
   </si>
   <si>
     <t xml:space="preserve">Sorgos</t>
@@ -673,7 +724,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -681,7 +732,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -706,10 +757,10 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="17.14"/>
@@ -755,40 +806,81 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="E2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="4"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D4" s="4"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="0" t="n">
+        <v>37508000</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="2"/>
+      <c r="C12" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -801,6 +893,9 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="email@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -819,10 +914,10 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.57"/>
@@ -838,63 +933,134 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J2" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>39.99</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>999</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="2"/>
+      <c r="I5" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -933,10 +1099,10 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13"/>
@@ -949,62 +1115,203 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>500.8</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>3200</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>2988.33</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>2700</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>3001.99</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1000.01</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="2"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="2"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -1042,7 +1349,7 @@
       <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.14"/>
@@ -1057,28 +1364,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
@@ -1086,604 +1393,604 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="2" t="n">
+        <v>34</v>
+      </c>
+      <c r="F2" s="3" t="n">
         <v>5101</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>51</v>
+        <v>77</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>58</v>
+        <v>82</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>64</v>
+        <v>87</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>68</v>
+        <v>91</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>72</v>
+        <v>95</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>76</v>
+        <v>99</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>80</v>
+        <v>54</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>84</v>
+        <v>106</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>88</v>
+        <v>109</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>92</v>
+        <v>113</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>96</v>
+        <v>117</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>100</v>
+        <v>121</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>104</v>
+        <v>125</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>122</v>
+        <v>143</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>130</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="0" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>136</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>137</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>139</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
-        <v>145</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="0" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="0" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="0" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="0" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="0" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="0" t="s">
-        <v>159</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="0" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="0" t="s">
-        <v>161</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="0" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="0" t="s">
-        <v>163</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="0" t="s">
-        <v>164</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="0" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="0" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="0" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="0" t="s">
-        <v>168</v>
+        <v>186</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="0" t="s">
-        <v>169</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B72" s="0" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="0" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
-        <v>173</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B76" s="0" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B77" s="0" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B78" s="0" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="0" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B80" s="0" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="0" t="s">
-        <v>179</v>
+        <v>62</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="0" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>